<commit_message>
new json file and read the data in d3
</commit_message>
<xml_diff>
--- a/D3Framework/ProfileReport_DataFix_ver2.xlsx
+++ b/D3Framework/ProfileReport_DataFix_ver2.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\cs399\Final\D3Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AAA3DF-A2AB-4075-A221-04C8710929C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB237AE1-188C-4A8A-A710-B5519EA2EEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{34114B15-436F-4B2C-ADB2-A3749E4FAA01}"/>
   </bookViews>
   <sheets>
-    <sheet name="0~1" sheetId="2" r:id="rId1"/>
-    <sheet name="1~2" sheetId="3" r:id="rId2"/>
-    <sheet name="2~3" sheetId="4" r:id="rId3"/>
-    <sheet name="3~4" sheetId="5" r:id="rId4"/>
-    <sheet name="4~5" sheetId="6" r:id="rId5"/>
-    <sheet name="5~6" sheetId="7" r:id="rId6"/>
-    <sheet name="6~7" sheetId="8" r:id="rId7"/>
-    <sheet name="7~8" sheetId="9" r:id="rId8"/>
-    <sheet name="8~9" sheetId="10" r:id="rId9"/>
-    <sheet name="9~10" sheetId="11" r:id="rId10"/>
+    <sheet name="one" sheetId="2" r:id="rId1"/>
+    <sheet name="two" sheetId="3" r:id="rId2"/>
+    <sheet name="three" sheetId="4" r:id="rId3"/>
+    <sheet name="four" sheetId="5" r:id="rId4"/>
+    <sheet name="five" sheetId="6" r:id="rId5"/>
+    <sheet name="six" sheetId="7" r:id="rId6"/>
+    <sheet name="seven" sheetId="8" r:id="rId7"/>
+    <sheet name="eight" sheetId="9" r:id="rId8"/>
+    <sheet name="nine" sheetId="10" r:id="rId9"/>
+    <sheet name="ten" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,26 +42,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="42">
-  <si>
-    <t>Time interval</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="49">
   <si>
     <t>Function</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hit Count</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Time(ms)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Index</t>
-  </si>
-  <si>
     <t>0~1</t>
   </si>
   <si>
@@ -156,10 +141,6 @@
   </si>
   <si>
     <t>9~10</t>
-  </si>
-  <si>
-    <t>Time / Hit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0~1</t>
@@ -171,6 +152,58 @@
   </si>
   <si>
     <t>b2ParticleSystem::UpdateBodyContacts'::`2'::UpdateBodyContactsCallback::ReportFixtureAndParticle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeHit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeInterval</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HitCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HitCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -537,9 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DFB4B4-57A3-445C-ACDA-5741269A646E}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -548,33 +579,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>191</v>
@@ -595,10 +626,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>105</v>
@@ -619,10 +650,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -643,10 +674,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>24</v>
@@ -667,10 +698,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -691,10 +722,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -715,10 +746,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -739,10 +770,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -763,10 +794,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -787,10 +818,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -823,40 +854,40 @@
   <dimension ref="O1:U11"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y7" sqref="Y7"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O1" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" t="s">
-        <v>1</v>
-      </c>
       <c r="Q1" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="R1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="S1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="T1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="U1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="Q2">
         <v>264</v>
@@ -877,10 +908,10 @@
     </row>
     <row r="3" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Q3">
         <v>34</v>
@@ -901,10 +932,10 @@
     </row>
     <row r="4" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="Q4">
         <v>22</v>
@@ -925,10 +956,10 @@
     </row>
     <row r="5" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="Q5">
         <v>11</v>
@@ -949,10 +980,10 @@
     </row>
     <row r="6" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="Q6">
         <v>9</v>
@@ -973,10 +1004,10 @@
     </row>
     <row r="7" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q7">
         <v>9</v>
@@ -997,10 +1028,10 @@
     </row>
     <row r="8" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="Q8">
         <v>9</v>
@@ -1021,10 +1052,10 @@
     </row>
     <row r="9" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q9">
         <v>8</v>
@@ -1045,10 +1076,10 @@
     </row>
     <row r="10" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P10" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q10">
         <v>7</v>
@@ -1069,10 +1100,10 @@
     </row>
     <row r="11" spans="15:21" x14ac:dyDescent="0.3">
       <c r="O11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="P11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="Q11">
         <v>7</v>
@@ -1105,40 +1136,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>232</v>
@@ -1159,10 +1190,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>18</v>
@@ -1183,10 +1214,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -1207,10 +1238,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -1231,10 +1262,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -1255,10 +1286,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>13</v>
@@ -1279,10 +1310,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -1303,10 +1334,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>12</v>
@@ -1327,10 +1358,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -1351,10 +1382,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -1387,40 +1418,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>213</v>
@@ -1441,10 +1472,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>17</v>
@@ -1465,10 +1496,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>17</v>
@@ -1489,10 +1520,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>17</v>
@@ -1513,10 +1544,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>15</v>
@@ -1537,10 +1568,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <v>14</v>
@@ -1561,10 +1592,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -1585,10 +1616,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>13</v>
@@ -1609,10 +1640,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>12</v>
@@ -1633,10 +1664,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <v>8</v>
@@ -1669,40 +1700,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A12:G71"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>224</v>
@@ -1723,10 +1754,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>39</v>
@@ -1747,10 +1778,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>32</v>
@@ -1771,10 +1802,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>19</v>
@@ -1795,10 +1826,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -1819,10 +1850,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -1843,10 +1874,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -1867,10 +1898,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>10</v>
@@ -1891,10 +1922,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -1915,10 +1946,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>9</v>
@@ -1951,40 +1982,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD65"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>260</v>
@@ -2005,10 +2036,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>41</v>
@@ -2029,10 +2060,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -2053,10 +2084,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>11</v>
@@ -2077,10 +2108,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -2101,10 +2132,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -2125,10 +2156,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -2149,10 +2180,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -2173,10 +2204,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -2197,10 +2228,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -2233,40 +2264,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD70"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>235</v>
@@ -2287,10 +2318,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>43</v>
@@ -2311,10 +2342,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -2335,10 +2366,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -2359,10 +2390,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -2383,10 +2414,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -2407,10 +2438,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -2431,10 +2462,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>11</v>
@@ -2455,10 +2486,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>10</v>
@@ -2479,10 +2510,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -2515,40 +2546,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD63"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>276</v>
@@ -2569,10 +2600,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>37</v>
@@ -2593,10 +2624,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -2617,10 +2648,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>14</v>
@@ -2641,10 +2672,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -2665,10 +2696,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -2689,10 +2720,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -2713,10 +2744,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -2737,10 +2768,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -2761,10 +2792,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -2797,40 +2828,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD64"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>279</v>
@@ -2851,10 +2882,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>39</v>
@@ -2875,10 +2906,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>16</v>
@@ -2899,10 +2930,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -2923,10 +2954,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -2947,10 +2978,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -2971,10 +3002,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>8</v>
@@ -2995,10 +3026,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>7</v>
@@ -3019,10 +3050,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>7</v>
@@ -3043,10 +3074,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -3079,40 +3110,40 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD63"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>257</v>
@@ -3133,10 +3164,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>39</v>
@@ -3157,10 +3188,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -3181,10 +3212,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>17</v>
@@ -3205,10 +3236,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6">
         <v>13</v>
@@ -3229,10 +3260,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -3253,10 +3284,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -3277,10 +3308,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -3301,10 +3332,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -3325,10 +3356,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>9</v>

</xml_diff>